<commit_message>
excel file percentage profit fixed
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dogru\Desktop\Github\BinancePortfolioTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109427D2-D0C7-4802-95A6-93EFD4714F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B0977C-91E6-4716-A0DC-C84C5558D212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,7 +199,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -211,6 +210,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,7 +537,7 @@
   <dimension ref="A1:XFC21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +548,7 @@
     <col min="4" max="4" width="18.140625" style="6" customWidth="1"/>
     <col min="5" max="6" width="17" style="6" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="13" customWidth="1"/>
     <col min="9" max="9" width="23.85546875" style="6" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" style="6" customWidth="1"/>
     <col min="11" max="11" width="17.85546875" style="6" customWidth="1"/>
@@ -561,38 +561,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -623,7 +623,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -638,7 +638,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="12"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -667,7 +667,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -682,7 +682,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="13"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>

</xml_diff>